<commit_message>
Fixed Error: "Cannot locate element with text: Mexico"
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/CreditCardsData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/CreditCardsData.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">08</t>
   </si>
   <si>
-    <t xml:space="preserve">Mexico</t>
+    <t xml:space="preserve">MX</t>
   </si>
   <si>
     <t xml:space="preserve">VISA</t>
@@ -208,7 +208,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>